<commit_message>
ispravljen unos u dnevnik
</commit_message>
<xml_diff>
--- a/DnevniciProjekta/Sonar_Dnevnik_Nebojsa_Zoraja_IT38_2019.xlsx
+++ b/DnevniciProjekta/Sonar_Dnevnik_Nebojsa_Zoraja_IT38_2019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Faks\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faks\Documents\Tim-1---Indijanci---NewDevProject\DnevniciProjekta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BED215-EE81-4403-9CA6-4963CAAE7477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF27711-72BE-41FA-A055-4B8DE9C9AD14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="2280" windowWidth="21600" windowHeight="11295" xr2:uid="{20C5DEC2-B10F-44F9-9ED1-5DB010ECB74B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20C5DEC2-B10F-44F9-9ED1-5DB010ECB74B}"/>
   </bookViews>
   <sheets>
     <sheet name="Diary" sheetId="1" r:id="rId1"/>
@@ -333,9 +333,6 @@
     <t>Unused asignment</t>
   </si>
   <si>
-    <t>Deleted unused object</t>
-  </si>
-  <si>
     <t>S1116</t>
   </si>
   <si>
@@ -343,6 +340,9 @@
   </si>
   <si>
     <t>Deleted redundant semicolon</t>
+  </si>
+  <si>
+    <t>Added a dto to use with mapper</t>
   </si>
 </sst>
 </file>
@@ -793,6 +793,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -820,7 +821,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1139,7 +1139,7 @@
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,52 +1158,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="28"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="31"/>
     </row>
     <row r="4" spans="1:12" ht="57.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
@@ -1247,7 +1247,7 @@
       <c r="A5" s="7">
         <v>44975</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="22" t="s">
         <v>45</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -1345,7 +1345,7 @@
         <v>28</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="J7" s="10" t="s">
         <v>21</v>
@@ -1362,7 +1362,7 @@
         <v>44975</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>9</v>
@@ -1374,7 +1374,7 @@
         <v>31</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="16">
         <v>1</v>
@@ -1383,7 +1383,7 @@
         <v>28</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J8" s="10" t="s">
         <v>21</v>

</xml_diff>